<commit_message>
Upgrade to content with actual poems
</commit_message>
<xml_diff>
--- a/jsClass/Poems.xlsx
+++ b/jsClass/Poems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1168,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1370,7 +1374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1475,7 +1481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1597,7 +1605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1719,7 +1729,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1844,7 +1856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1985,7 +1999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2112,7 +2128,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>